<commit_message>
DDFramework - add LoginTest with DataProvider from Excel file
</commit_message>
<xml_diff>
--- a/DDFramework1/resources/excel/testdata.xlsx
+++ b/DDFramework1/resources/excel/testdata.xlsx
@@ -20,46 +20,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">username</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">email</t>
   </si>
   <si>
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">is_correct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">citrue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">many</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pepa</t>
+    <t xml:space="preserve">message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid Email or Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demouser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user@phptravels.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi, Demo User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -83,6 +81,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,11 +147,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -168,17 +172,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -194,58 +198,90 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>111</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>222</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="n">
-        <v>333</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>444</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>555</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DDFramework - add more TCs, methods and optimize framework
</commit_message>
<xml_diff>
--- a/DDFramework1/resources/excel/testdata.xlsx
+++ b/DDFramework1/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -180,7 +180,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>

</xml_diff>